<commit_message>
Creacion de metodos CRUD en Generico Configuracion de CRUD en repositorio Generico Diseño Pantalla de Login
</commit_message>
<xml_diff>
--- a/Plantilla Project Plan.xlsx
+++ b/Plantilla Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalcantara\source\repos\SAV - FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B3FC16-4E36-48BC-BAD7-973B6B4E76C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023B66EA-0B33-4C43-A9DB-BD1D6771A224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F35EB38B-CF59-904E-A07C-A9DF5B998A26}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>Order</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>1, 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Creacion de metodos CRUD en Generico</t>
+  </si>
+  <si>
+    <t>Configuracion de CRUD en repositorio Generico</t>
+  </si>
+  <si>
+    <t>Configuracion de la pantalla de Login</t>
+  </si>
+  <si>
+    <t>Diseño Pantalla de Login</t>
   </si>
 </sst>
 </file>
@@ -549,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D065043C-E85A-734C-A604-A2CC30561E94}">
-  <dimension ref="A1:I287"/>
+  <dimension ref="A1:I291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -568,7 +580,7 @@
     <col min="9" max="9" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -594,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -620,7 +632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -646,7 +658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -672,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -698,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -724,7 +736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -750,7 +762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -776,7 +788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -795,131 +807,97 @@
       <c r="F9" s="6">
         <v>44423</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="G9" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6">
+        <v>44427</v>
+      </c>
+      <c r="F10" s="6">
+        <v>44427</v>
+      </c>
+      <c r="G10" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="6">
-        <v>44423</v>
-      </c>
-      <c r="F10" s="6">
-        <v>44423</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="6">
-        <v>44424</v>
-      </c>
-      <c r="F11" s="6">
-        <v>44426</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="6">
-        <v>44424</v>
-      </c>
-      <c r="F12" s="6">
-        <v>44426</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="6">
-        <v>44426</v>
-      </c>
-      <c r="F13" s="6">
-        <v>44427</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="6">
-        <v>44426</v>
+        <v>44423</v>
       </c>
       <c r="F14" s="6">
-        <v>44427</v>
+        <v>44423</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>32</v>
@@ -928,23 +906,20 @@
         <v>15</v>
       </c>
       <c r="E15" s="6">
-        <v>44428</v>
+        <v>44424</v>
       </c>
       <c r="F15" s="6">
-        <v>44428</v>
+        <v>44426</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>32</v>
@@ -953,21 +928,20 @@
         <v>30</v>
       </c>
       <c r="E16" s="6">
-        <v>44428</v>
+        <v>44424</v>
       </c>
       <c r="F16" s="6">
-        <v>44428</v>
+        <v>44426</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>32</v>
@@ -976,97 +950,155 @@
         <v>15</v>
       </c>
       <c r="E17" s="6">
-        <v>44429</v>
+        <v>44426</v>
       </c>
       <c r="F17" s="6">
-        <v>44430</v>
+        <v>44427</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E18" s="6">
-        <v>44430</v>
+        <v>44426</v>
       </c>
       <c r="F18" s="6">
-        <v>44432</v>
+        <v>44427</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="6">
+        <v>44428</v>
+      </c>
+      <c r="F19" s="6">
+        <v>44428</v>
+      </c>
+      <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="I19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="6">
+        <v>44428</v>
+      </c>
+      <c r="F20" s="6">
+        <v>44428</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>16</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="6">
+        <v>44429</v>
+      </c>
+      <c r="F21" s="6">
+        <v>44430</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="6">
+        <v>44430</v>
+      </c>
+      <c r="F22" s="6">
+        <v>44432</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
+      <c r="E23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1076,7 +1108,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1086,7 +1118,7 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1096,7 +1128,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1106,7 +1138,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1116,7 +1148,7 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1126,7 +1158,7 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1136,7 +1168,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1146,7 +1178,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3706,14 +3738,54 @@
       <c r="G287" s="5"/>
       <c r="H287" s="5"/>
     </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A288" s="4"/>
+      <c r="B288" s="4"/>
+      <c r="C288" s="4"/>
+      <c r="D288" s="4"/>
+      <c r="E288" s="4"/>
+      <c r="F288" s="4"/>
+      <c r="G288" s="5"/>
+      <c r="H288" s="5"/>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A289" s="4"/>
+      <c r="B289" s="4"/>
+      <c r="C289" s="4"/>
+      <c r="D289" s="4"/>
+      <c r="E289" s="4"/>
+      <c r="F289" s="4"/>
+      <c r="G289" s="5"/>
+      <c r="H289" s="5"/>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A290" s="4"/>
+      <c r="B290" s="4"/>
+      <c r="C290" s="4"/>
+      <c r="D290" s="4"/>
+      <c r="E290" s="4"/>
+      <c r="F290" s="4"/>
+      <c r="G290" s="5"/>
+      <c r="H290" s="5"/>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A291" s="4"/>
+      <c r="B291" s="4"/>
+      <c r="C291" s="4"/>
+      <c r="D291" s="4"/>
+      <c r="E291" s="4"/>
+      <c r="F291" s="4"/>
+      <c r="G291" s="5"/>
+      <c r="H291" s="5"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I13:I15">
-    <sortCondition ref="I13:I15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I17:I19">
+    <sortCondition ref="I17:I19"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H287" xr:uid="{178FC5F2-D507-004B-AAAB-2C2E3F32C46E}">
-      <formula1>$I$12:$I$15</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H291" xr:uid="{178FC5F2-D507-004B-AAAB-2C2E3F32C46E}">
+      <formula1>$I$16:$I$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creacion de metodos CRUD en Generico Configuracion de CRUD en repositorio Generico Diseño Pantalla de Login Configuracion de la pantalla de Login Diseño Pantalla de Usuario Configuracion Metodo Buscar todos los Usuarios Configuracion Metodo Crear Usuario
</commit_message>
<xml_diff>
--- a/Plantilla Project Plan.xlsx
+++ b/Plantilla Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalcantara\source\repos\SAV - FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023B66EA-0B33-4C43-A9DB-BD1D6771A224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7F8983-C7E9-4507-BC89-54F8ABEAF849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F35EB38B-CF59-904E-A07C-A9DF5B998A26}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>Order</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Diseño Pantalla de Login</t>
+  </si>
+  <si>
+    <t>Diseño Pantalla de Usuario</t>
+  </si>
+  <si>
+    <t>Configuracion Metodo Crear Usuario</t>
+  </si>
+  <si>
+    <t>Configuracion Metodo Buscar todos los Usuarios</t>
   </si>
 </sst>
 </file>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D065043C-E85A-734C-A604-A2CC30561E94}">
-  <dimension ref="A1:I291"/>
+  <dimension ref="A1:I294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -820,7 +829,9 @@
         <v>38</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E10" s="6">
         <v>44427</v>
       </c>
@@ -840,11 +851,21 @@
         <v>39</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="5"/>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6">
+        <v>44427</v>
+      </c>
+      <c r="F11" s="6">
+        <v>44427</v>
+      </c>
+      <c r="G11" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -852,11 +873,21 @@
         <v>41</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="6">
+        <v>44427</v>
+      </c>
+      <c r="F12" s="6">
+        <v>44427</v>
+      </c>
+      <c r="G12" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -864,268 +895,314 @@
         <v>40</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="5"/>
+      <c r="D13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="6">
+        <v>44427</v>
+      </c>
+      <c r="F13" s="6">
+        <v>44427</v>
+      </c>
+      <c r="G13" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>9</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="6">
-        <v>44423</v>
+        <v>44427</v>
       </c>
       <c r="F14" s="6">
-        <v>44423</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>44427</v>
+      </c>
+      <c r="G14" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>10</v>
-      </c>
+      <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="6">
-        <v>44424</v>
+        <v>44427</v>
       </c>
       <c r="F15" s="6">
-        <v>44426</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+        <v>44427</v>
+      </c>
+      <c r="G15" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>11</v>
-      </c>
+      <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E16" s="6">
-        <v>44424</v>
+        <v>44427</v>
       </c>
       <c r="F16" s="6">
-        <v>44426</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+        <v>44427</v>
+      </c>
+      <c r="G16" s="6">
+        <v>44427</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E17" s="6">
-        <v>44426</v>
+        <v>44423</v>
       </c>
       <c r="F17" s="6">
-        <v>44427</v>
+        <v>44423</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E18" s="6">
+        <v>44424</v>
+      </c>
+      <c r="F18" s="6">
         <v>44426</v>
-      </c>
-      <c r="F18" s="6">
-        <v>44427</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6">
-        <v>44428</v>
+        <v>44424</v>
       </c>
       <c r="F19" s="6">
-        <v>44428</v>
+        <v>44426</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E20" s="6">
-        <v>44428</v>
+        <v>44426</v>
       </c>
       <c r="F20" s="6">
-        <v>44428</v>
+        <v>44427</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E21" s="6">
-        <v>44429</v>
+        <v>44426</v>
       </c>
       <c r="F21" s="6">
-        <v>44430</v>
+        <v>44427</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
+      <c r="I21" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E22" s="6">
-        <v>44430</v>
+        <v>44428</v>
       </c>
       <c r="F22" s="6">
-        <v>44432</v>
+        <v>44428</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
+      <c r="I22" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="6">
+        <v>44428</v>
+      </c>
+      <c r="F23" s="6">
+        <v>44428</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="A24" s="4">
+        <v>16</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="6">
+        <v>44429</v>
+      </c>
+      <c r="F24" s="6">
+        <v>44430</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="A25" s="4">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="6">
+        <v>44430</v>
+      </c>
+      <c r="F25" s="6">
+        <v>44432</v>
+      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="4">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
+      <c r="E26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3778,14 +3855,44 @@
       <c r="G291" s="5"/>
       <c r="H291" s="5"/>
     </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A292" s="4"/>
+      <c r="B292" s="4"/>
+      <c r="C292" s="4"/>
+      <c r="D292" s="4"/>
+      <c r="E292" s="4"/>
+      <c r="F292" s="4"/>
+      <c r="G292" s="5"/>
+      <c r="H292" s="5"/>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A293" s="4"/>
+      <c r="B293" s="4"/>
+      <c r="C293" s="4"/>
+      <c r="D293" s="4"/>
+      <c r="E293" s="4"/>
+      <c r="F293" s="4"/>
+      <c r="G293" s="5"/>
+      <c r="H293" s="5"/>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A294" s="4"/>
+      <c r="B294" s="4"/>
+      <c r="C294" s="4"/>
+      <c r="D294" s="4"/>
+      <c r="E294" s="4"/>
+      <c r="F294" s="4"/>
+      <c r="G294" s="5"/>
+      <c r="H294" s="5"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I17:I19">
-    <sortCondition ref="I17:I19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I20:I22">
+    <sortCondition ref="I20:I22"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H291" xr:uid="{178FC5F2-D507-004B-AAAB-2C2E3F32C46E}">
-      <formula1>$I$16:$I$19</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H294" xr:uid="{178FC5F2-D507-004B-AAAB-2C2E3F32C46E}">
+      <formula1>$I$19:$I$22</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>